<commit_message>
valid visual formating for xlxs
</commit_message>
<xml_diff>
--- a/fontstyle.xlsx
+++ b/fontstyle.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="472">
   <si>
     <t>Release Date:</t>
   </si>
@@ -39,7 +39,7 @@
     <t>Author:</t>
   </si>
   <si>
-    <t>JLyc</t>
+    <t>sochaa</t>
   </si>
   <si>
     <t>List of artefacts to be provided for cutover</t>
@@ -1439,7 +1439,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -1468,13 +1468,33 @@
       <sz val="11.0"/>
       <b val="true"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C0C0C0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1492,7 +1512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyBorder="true" applyFont="true"/>
@@ -1782,7 +1802,9 @@
       <alignment wrapText="true" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -4325,6 +4347,13 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="9" max="9" width="40.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3.90625" customWidth="true"/>
+    <col min="2" max="2" width="3.90625" customWidth="true"/>
+    <col min="3" max="3" width="3.90625" customWidth="true"/>
+    <col min="4" max="4" width="3.90625" customWidth="true"/>
+    <col min="5" max="5" width="3.90625" customWidth="true"/>
+    <col min="6" max="6" width="3.90625" customWidth="true"/>
+    <col min="7" max="7" width="3.90625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4347,37 +4376,37 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="99">
         <v>248</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="99">
         <v>249</v>
       </c>
     </row>
     <row r="6">
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="99">
         <v>250</v>
       </c>
     </row>
     <row r="7">
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="99">
         <v>251</v>
       </c>
     </row>
     <row r="8">
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="99">
         <v>252</v>
       </c>
     </row>
     <row r="9">
-      <c r="F9" t="s">
+      <c r="F9" t="s" s="99">
         <v>241</v>
       </c>
     </row>
     <row r="10">
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="99">
         <v>253</v>
       </c>
     </row>
@@ -4390,7 +4419,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="G12" t="s">
+      <c r="G12" t="s" s="99">
         <v>256</v>
       </c>
     </row>
@@ -4403,17 +4432,17 @@
       </c>
     </row>
     <row r="14">
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="99">
         <v>258</v>
       </c>
     </row>
     <row r="15">
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="99">
         <v>259</v>
       </c>
     </row>
     <row r="16">
-      <c r="F16" t="s">
+      <c r="F16" t="s" s="99">
         <v>260</v>
       </c>
     </row>
@@ -4434,7 +4463,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="99">
         <v>263</v>
       </c>
     </row>
@@ -4463,32 +4492,32 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="99">
         <v>267</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="99">
         <v>249</v>
       </c>
     </row>
     <row r="25">
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="99">
         <v>268</v>
       </c>
     </row>
     <row r="26">
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="99">
         <v>251</v>
       </c>
     </row>
     <row r="27">
-      <c r="E27" t="s">
+      <c r="E27" t="s" s="99">
         <v>252</v>
       </c>
     </row>
     <row r="28">
-      <c r="F28" t="s">
+      <c r="F28" t="s" s="99">
         <v>241</v>
       </c>
     </row>
@@ -4501,7 +4530,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="G30" t="s">
+      <c r="G30" t="s" s="99">
         <v>270</v>
       </c>
     </row>
@@ -4514,7 +4543,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="G32" t="s">
+      <c r="G32" t="s" s="99">
         <v>256</v>
       </c>
     </row>
@@ -4535,17 +4564,17 @@
       </c>
     </row>
     <row r="35">
-      <c r="D35" t="s">
+      <c r="D35" t="s" s="99">
         <v>258</v>
       </c>
     </row>
     <row r="36">
-      <c r="E36" t="s">
+      <c r="E36" t="s" s="99">
         <v>259</v>
       </c>
     </row>
     <row r="37">
-      <c r="F37" t="s">
+      <c r="F37" t="s" s="99">
         <v>274</v>
       </c>
     </row>
@@ -4566,7 +4595,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="99">
         <v>263</v>
       </c>
     </row>
@@ -4595,32 +4624,32 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
+      <c r="A44" t="s" s="99">
         <v>277</v>
       </c>
     </row>
     <row r="45">
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="99">
         <v>249</v>
       </c>
     </row>
     <row r="46">
-      <c r="C46" t="s">
+      <c r="C46" t="s" s="99">
         <v>278</v>
       </c>
     </row>
     <row r="47">
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="99">
         <v>279</v>
       </c>
     </row>
     <row r="48">
-      <c r="E48" t="s">
+      <c r="E48" t="s" s="99">
         <v>280</v>
       </c>
     </row>
     <row r="49">
-      <c r="F49" t="s">
+      <c r="F49" t="s" s="99">
         <v>281</v>
       </c>
     </row>
@@ -4633,7 +4662,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="F51" t="s">
+      <c r="F51" t="s" s="99">
         <v>283</v>
       </c>
     </row>
@@ -4646,7 +4675,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="F53" t="s">
+      <c r="F53" t="s" s="99">
         <v>285</v>
       </c>
     </row>
@@ -4659,7 +4688,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="F55" t="s">
+      <c r="F55" t="s" s="99">
         <v>256</v>
       </c>
     </row>
@@ -4696,17 +4725,17 @@
       </c>
     </row>
     <row r="60">
-      <c r="D60" t="s">
+      <c r="D60" t="s" s="99">
         <v>291</v>
       </c>
     </row>
     <row r="61">
-      <c r="E61" t="s">
+      <c r="E61" t="s" s="99">
         <v>292</v>
       </c>
     </row>
     <row r="62">
-      <c r="F62" t="s">
+      <c r="F62" t="s" s="99">
         <v>293</v>
       </c>
     </row>
@@ -4719,7 +4748,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="F64" t="s">
+      <c r="F64" t="s" s="99">
         <v>295</v>
       </c>
     </row>
@@ -4748,7 +4777,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="F68" t="s">
+      <c r="F68" t="s" s="99">
         <v>299</v>
       </c>
     </row>
@@ -4769,7 +4798,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="F71" t="s">
+      <c r="F71" t="s" s="99">
         <v>302</v>
       </c>
     </row>
@@ -4790,7 +4819,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="F74" t="s">
+      <c r="F74" t="s" s="99">
         <v>256</v>
       </c>
     </row>
@@ -4867,17 +4896,17 @@
       </c>
     </row>
     <row r="84">
-      <c r="D84" t="s">
+      <c r="D84" t="s" s="99">
         <v>314</v>
       </c>
     </row>
     <row r="85">
-      <c r="E85" t="s">
+      <c r="E85" t="s" s="99">
         <v>235</v>
       </c>
     </row>
     <row r="86">
-      <c r="F86" t="s">
+      <c r="F86" t="s" s="99">
         <v>315</v>
       </c>
     </row>
@@ -4890,7 +4919,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="F88" t="s">
+      <c r="F88" t="s" s="99">
         <v>317</v>
       </c>
     </row>
@@ -4903,7 +4932,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="F90" t="s">
+      <c r="F90" t="s" s="99">
         <v>319</v>
       </c>
     </row>
@@ -4916,7 +4945,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="F92" t="s">
+      <c r="F92" t="s" s="99">
         <v>321</v>
       </c>
     </row>
@@ -4929,7 +4958,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="F94" t="s">
+      <c r="F94" t="s" s="99">
         <v>256</v>
       </c>
     </row>
@@ -4974,7 +5003,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="E100" t="s">
+      <c r="E100" t="s" s="99">
         <v>328</v>
       </c>
     </row>
@@ -4995,17 +5024,17 @@
       </c>
     </row>
     <row r="103">
-      <c r="D103" t="s">
+      <c r="D103" t="s" s="99">
         <v>331</v>
       </c>
     </row>
     <row r="104">
-      <c r="E104" t="s">
+      <c r="E104" t="s" s="99">
         <v>332</v>
       </c>
     </row>
     <row r="105">
-      <c r="F105" t="s">
+      <c r="F105" t="s" s="99">
         <v>333</v>
       </c>
     </row>
@@ -5018,7 +5047,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="F107" t="s">
+      <c r="F107" t="s" s="99">
         <v>335</v>
       </c>
     </row>
@@ -5031,7 +5060,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="F109" t="s">
+      <c r="F109" t="s" s="99">
         <v>337</v>
       </c>
     </row>
@@ -5044,7 +5073,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="F111" t="s">
+      <c r="F111" t="s" s="99">
         <v>321</v>
       </c>
     </row>
@@ -5057,7 +5086,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="F113" t="s">
+      <c r="F113" t="s" s="99">
         <v>339</v>
       </c>
     </row>
@@ -5070,7 +5099,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="F115" t="s">
+      <c r="F115" t="s" s="99">
         <v>256</v>
       </c>
     </row>
@@ -5123,12 +5152,12 @@
       </c>
     </row>
     <row r="122">
-      <c r="D122" t="s">
+      <c r="D122" t="s" s="99">
         <v>344</v>
       </c>
     </row>
     <row r="123">
-      <c r="E123" t="s">
+      <c r="E123" t="s" s="99">
         <v>345</v>
       </c>
     </row>
@@ -5141,7 +5170,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="F125" t="s">
+      <c r="F125" t="s" s="99">
         <v>346</v>
       </c>
     </row>
@@ -5154,7 +5183,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="F127" t="s">
+      <c r="F127" t="s" s="99">
         <v>348</v>
       </c>
     </row>
@@ -5167,7 +5196,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="F129" t="s">
+      <c r="F129" t="s" s="99">
         <v>350</v>
       </c>
     </row>
@@ -5180,7 +5209,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="F131" t="s">
+      <c r="F131" t="s" s="99">
         <v>352</v>
       </c>
     </row>
@@ -5193,7 +5222,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="F133" t="s">
+      <c r="F133" t="s" s="99">
         <v>354</v>
       </c>
     </row>
@@ -5206,7 +5235,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="F135" t="s">
+      <c r="F135" t="s" s="99">
         <v>256</v>
       </c>
     </row>
@@ -5259,17 +5288,17 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="s">
+      <c r="A142" t="s" s="99">
         <v>362</v>
       </c>
     </row>
     <row r="143">
-      <c r="B143" t="s">
+      <c r="B143" t="s" s="99">
         <v>363</v>
       </c>
     </row>
     <row r="144">
-      <c r="C144" t="s">
+      <c r="C144" t="s" s="99">
         <v>364</v>
       </c>
     </row>
@@ -5282,7 +5311,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="D146" t="s">
+      <c r="D146" t="s" s="99">
         <v>366</v>
       </c>
     </row>
@@ -5327,7 +5356,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="C152" t="s">
+      <c r="C152" t="s" s="99">
         <v>372</v>
       </c>
     </row>
@@ -5420,7 +5449,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="C164" t="s">
+      <c r="C164" t="s" s="99">
         <v>384</v>
       </c>
     </row>
@@ -5441,7 +5470,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="C167" t="s">
+      <c r="C167" t="s" s="99">
         <v>387</v>
       </c>
     </row>
@@ -5502,7 +5531,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="B175" t="s">
+      <c r="B175" t="s" s="99">
         <v>395</v>
       </c>
     </row>
@@ -5539,7 +5568,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="B180" t="s">
+      <c r="B180" t="s" s="99">
         <v>400</v>
       </c>
     </row>
@@ -5608,7 +5637,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="C189" t="s">
+      <c r="C189" t="s" s="99">
         <v>408</v>
       </c>
     </row>
@@ -5761,7 +5790,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="97.265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="99.73046875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="40.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -5773,1433 +5802,1646 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="99" customFormat="true">
-      <c r="A3" t="s" s="99">
+    <row r="3" s="100" customFormat="true">
+      <c r="A3" t="s" s="100">
         <v>246</v>
       </c>
-      <c r="B3" t="s" s="99">
+      <c r="B3" t="s" s="100">
         <v>247</v>
       </c>
-      <c r="C3" t="s" s="99">
+      <c r="C3" t="s" s="100">
         <v>25</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" t="s" s="101">
         <v>426</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
         <v>254</v>
       </c>
-      <c r="C4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="C6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" t="s" s="101">
         <v>427</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
         <v>257</v>
       </c>
-      <c r="C5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="C9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11">
+      <c r="A11" t="s" s="101">
         <v>428</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
         <v>261</v>
       </c>
-      <c r="C6" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>428</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
         <v>262</v>
       </c>
-      <c r="C7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
+      <c r="C13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15">
+      <c r="A15" t="s" s="101">
         <v>429</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
         <v>264</v>
       </c>
-      <c r="C8" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>429</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
         <v>265</v>
       </c>
-      <c r="C9" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>429</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
         <v>266</v>
       </c>
-      <c r="C10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
+      <c r="C18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" t="s" s="101">
         <v>430</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B20" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
         <v>269</v>
       </c>
-      <c r="C11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
+      <c r="C21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22"/>
+    <row r="23">
+      <c r="A23" t="s" s="101">
         <v>431</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B23" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
         <v>271</v>
       </c>
-      <c r="C12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
+      <c r="C24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25"/>
+    <row r="26">
+      <c r="A26" t="s" s="101">
         <v>432</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B26" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
         <v>272</v>
       </c>
-      <c r="C13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>432</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
         <v>273</v>
       </c>
-      <c r="C14" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
+      <c r="C28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29"/>
+    <row r="30">
+      <c r="A30" t="s" s="101">
         <v>433</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B30" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
         <v>275</v>
       </c>
-      <c r="C15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>433</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
         <v>276</v>
       </c>
-      <c r="C16" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
+      <c r="C32" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33"/>
+    <row r="34">
+      <c r="A34" t="s" s="101">
         <v>434</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B34" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
         <v>264</v>
       </c>
-      <c r="C17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>434</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
         <v>265</v>
       </c>
-      <c r="C18" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>434</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
         <v>266</v>
       </c>
-      <c r="C19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
+      <c r="C37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38"/>
+    <row r="39">
+      <c r="A39" t="s" s="101">
         <v>435</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B39" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
         <v>282</v>
       </c>
-      <c r="C20" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
+      <c r="C40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41"/>
+    <row r="42">
+      <c r="A42" t="s" s="101">
         <v>436</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B42" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
         <v>284</v>
       </c>
-      <c r="C21" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
+      <c r="C43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45">
+      <c r="A45" t="s" s="101">
         <v>437</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B45" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
         <v>286</v>
       </c>
-      <c r="C22" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
+      <c r="C46" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="47"/>
+    <row r="48">
+      <c r="A48" t="s" s="101">
         <v>438</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B48" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
         <v>287</v>
       </c>
-      <c r="C23" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>438</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C49" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
         <v>288</v>
       </c>
-      <c r="C24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>438</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
         <v>289</v>
       </c>
-      <c r="C25" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>438</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
         <v>290</v>
       </c>
-      <c r="C26" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
+      <c r="C52" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53"/>
+    <row r="54">
+      <c r="A54" t="s" s="101">
         <v>439</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B54" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
         <v>294</v>
       </c>
-      <c r="C27" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
+      <c r="C55" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56"/>
+    <row r="57">
+      <c r="A57" t="s" s="101">
         <v>440</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B57" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
         <v>296</v>
       </c>
-      <c r="C28" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
+      <c r="C58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59"/>
+    <row r="60">
+      <c r="A60" t="s" s="101">
         <v>441</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B60" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
         <v>297</v>
       </c>
-      <c r="C29" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
+      <c r="C61" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>298</v>
+      </c>
+      <c r="C62" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63"/>
+    <row r="64">
+      <c r="A64" t="s" s="101">
+        <v>442</v>
+      </c>
+      <c r="B64" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>300</v>
+      </c>
+      <c r="C65" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="66"/>
+    <row r="67">
+      <c r="A67" t="s" s="101">
         <v>441</v>
       </c>
-      <c r="B30" t="s">
-        <v>298</v>
-      </c>
-      <c r="C30" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>442</v>
-      </c>
-      <c r="B31" t="s">
-        <v>300</v>
-      </c>
-      <c r="C31" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
+      <c r="B67" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>301</v>
+      </c>
+      <c r="C68" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="69"/>
+    <row r="70">
+      <c r="A70" t="s" s="101">
+        <v>443</v>
+      </c>
+      <c r="B70" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>303</v>
+      </c>
+      <c r="C71" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="72"/>
+    <row r="73">
+      <c r="A73" t="s" s="101">
         <v>441</v>
       </c>
-      <c r="B32" t="s">
-        <v>301</v>
-      </c>
-      <c r="C32" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>443</v>
-      </c>
-      <c r="B33" t="s">
-        <v>303</v>
-      </c>
-      <c r="C33" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>441</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="B73" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
         <v>304</v>
       </c>
-      <c r="C34" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
+      <c r="C74" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75"/>
+    <row r="76">
+      <c r="A76" t="s" s="101">
         <v>444</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B76" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
         <v>305</v>
       </c>
-      <c r="C35" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>444</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C77" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
         <v>306</v>
       </c>
-      <c r="C36" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>444</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C78" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
         <v>307</v>
       </c>
-      <c r="C37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>444</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C79" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
         <v>308</v>
       </c>
-      <c r="C38" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>444</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C80" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
         <v>309</v>
       </c>
-      <c r="C39" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>444</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C81" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
         <v>310</v>
       </c>
-      <c r="C40" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>444</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C82" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
         <v>311</v>
       </c>
-      <c r="C41" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>444</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C83" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
         <v>312</v>
       </c>
-      <c r="C42" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>444</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C84" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
         <v>313</v>
       </c>
-      <c r="C43" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
+      <c r="C85" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86"/>
+    <row r="87">
+      <c r="A87" t="s" s="101">
         <v>445</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B87" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
         <v>316</v>
       </c>
-      <c r="C44" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
+      <c r="C88" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="89"/>
+    <row r="90">
+      <c r="A90" t="s" s="101">
         <v>446</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B90" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
         <v>318</v>
       </c>
-      <c r="C45" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
+      <c r="C91" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92"/>
+    <row r="93">
+      <c r="A93" t="s" s="101">
         <v>447</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B93" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
         <v>320</v>
       </c>
-      <c r="C46" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
+      <c r="C94" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95"/>
+    <row r="96">
+      <c r="A96" t="s" s="101">
         <v>448</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B96" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
         <v>322</v>
       </c>
-      <c r="C47" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
+      <c r="C97" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="98"/>
+    <row r="99">
+      <c r="A99" t="s" s="101">
         <v>449</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B99" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
         <v>323</v>
       </c>
-      <c r="C48" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>449</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
         <v>324</v>
       </c>
-      <c r="C49" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>449</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C101" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
         <v>325</v>
       </c>
-      <c r="C50" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>449</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C102" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
         <v>326</v>
       </c>
-      <c r="C51" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>449</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C103" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
         <v>327</v>
       </c>
-      <c r="C52" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
+      <c r="C104" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="105"/>
+    <row r="106">
+      <c r="A106" t="s" s="101">
         <v>450</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B106" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="s">
         <v>329</v>
       </c>
-      <c r="C53" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>450</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C107" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" t="s">
         <v>330</v>
       </c>
-      <c r="C54" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
+      <c r="C108" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="109"/>
+    <row r="110">
+      <c r="A110" t="s" s="101">
         <v>451</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B110" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" t="s">
         <v>334</v>
       </c>
-      <c r="C55" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
+      <c r="C111" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="112"/>
+    <row r="113">
+      <c r="A113" t="s" s="101">
         <v>452</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B113" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="s">
         <v>336</v>
       </c>
-      <c r="C56" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
+      <c r="C114" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="115"/>
+    <row r="116">
+      <c r="A116" t="s" s="101">
         <v>453</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B116" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" t="s">
         <v>338</v>
       </c>
-      <c r="C57" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
+      <c r="C117" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="118"/>
+    <row r="119">
+      <c r="A119" t="s" s="101">
         <v>454</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B119" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" t="s">
         <v>322</v>
       </c>
-      <c r="C58" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
+      <c r="C120" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="121"/>
+    <row r="122">
+      <c r="A122" t="s" s="101">
         <v>455</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B122" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" t="s">
         <v>304</v>
       </c>
-      <c r="C59" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
+      <c r="C123" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="124"/>
+    <row r="125">
+      <c r="A125" t="s" s="101">
         <v>456</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B125" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" t="s">
         <v>340</v>
       </c>
-      <c r="C60" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>456</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C126" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" t="s">
         <v>341</v>
       </c>
-      <c r="C61" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>456</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C127" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" t="s">
         <v>342</v>
       </c>
-      <c r="C62" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>456</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C128" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="s">
         <v>343</v>
       </c>
-      <c r="C63" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>456</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C129" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="s">
         <v>327</v>
       </c>
-      <c r="C64" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>456</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C130" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="s">
         <v>313</v>
       </c>
-      <c r="C65" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
+      <c r="C131" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="132"/>
+    <row r="133">
+      <c r="A133" t="s" s="101">
         <v>457</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B133" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="s">
         <v>269</v>
       </c>
-      <c r="C66" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
+      <c r="C134" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="135"/>
+    <row r="136">
+      <c r="A136" t="s" s="101">
         <v>458</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B136" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="s">
         <v>347</v>
       </c>
-      <c r="C67" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
+      <c r="C137" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="138"/>
+    <row r="139">
+      <c r="A139" t="s" s="101">
         <v>459</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B139" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" t="s">
         <v>349</v>
       </c>
-      <c r="C68" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
+      <c r="C140" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="141"/>
+    <row r="142">
+      <c r="A142" t="s" s="101">
         <v>460</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B142" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" t="s">
         <v>351</v>
       </c>
-      <c r="C69" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
+      <c r="C143" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="144"/>
+    <row r="145">
+      <c r="A145" t="s" s="101">
         <v>461</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B145" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146" t="s">
         <v>353</v>
       </c>
-      <c r="C70" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
+      <c r="C146" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="147"/>
+    <row r="148">
+      <c r="A148" t="s" s="101">
         <v>462</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B148" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C148" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" t="s">
         <v>355</v>
       </c>
-      <c r="C71" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
+      <c r="C149" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="150"/>
+    <row r="151">
+      <c r="A151" t="s" s="101">
         <v>463</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B151" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="B152" t="s">
         <v>356</v>
       </c>
-      <c r="C72" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>463</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C152" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="B153" t="s">
         <v>357</v>
       </c>
-      <c r="C73" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>463</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C153" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="B154" t="s">
         <v>358</v>
       </c>
-      <c r="C74" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>463</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="C154" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="B155" t="s">
         <v>359</v>
       </c>
-      <c r="C75" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>463</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C155" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="B156" t="s">
         <v>360</v>
       </c>
-      <c r="C76" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>463</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="C156" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="B157" t="s">
         <v>361</v>
       </c>
-      <c r="C77" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
+      <c r="C157" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="158"/>
+    <row r="159">
+      <c r="A159" t="s" s="101">
         <v>464</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B159" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C159" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="B160" t="s">
         <v>365</v>
       </c>
-      <c r="C78" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
+      <c r="C160" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="161"/>
+    <row r="162">
+      <c r="A162" t="s" s="101">
         <v>465</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B162" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C162" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" t="s">
         <v>367</v>
       </c>
-      <c r="C79" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
+      <c r="C163" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="164"/>
+    <row r="165">
+      <c r="A165" t="s" s="101">
         <v>464</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B165" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" t="s">
         <v>368</v>
       </c>
-      <c r="C80" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>464</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="C166" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="s">
         <v>369</v>
       </c>
-      <c r="C81" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
-        <v>464</v>
-      </c>
-      <c r="B82" t="s">
+      <c r="C167" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" t="s">
         <v>370</v>
       </c>
-      <c r="C82" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>464</v>
-      </c>
-      <c r="B83" t="s">
+      <c r="C168" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" t="s">
         <v>371</v>
       </c>
-      <c r="C83" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
+      <c r="C169" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="170"/>
+    <row r="171">
+      <c r="A171" t="s" s="101">
         <v>466</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B171" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" t="s">
         <v>373</v>
       </c>
-      <c r="C84" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>466</v>
-      </c>
-      <c r="B85" t="s">
+      <c r="C172" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" t="s">
         <v>374</v>
       </c>
-      <c r="C85" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>466</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="C173" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="s">
         <v>375</v>
       </c>
-      <c r="C86" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>466</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="C174" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="s">
         <v>376</v>
       </c>
-      <c r="C87" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>466</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C175" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" t="s">
         <v>377</v>
       </c>
-      <c r="C88" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>466</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="C176" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" t="s">
         <v>378</v>
       </c>
-      <c r="C89" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>466</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="C177" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" t="s">
         <v>379</v>
       </c>
-      <c r="C90" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>466</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C178" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="B179" t="s">
         <v>380</v>
       </c>
-      <c r="C91" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>466</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="C179" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="s">
         <v>381</v>
       </c>
-      <c r="C92" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>466</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="C180" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="B181" t="s">
         <v>382</v>
       </c>
-      <c r="C93" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>466</v>
-      </c>
-      <c r="B94" t="s">
+      <c r="C181" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="B182" t="s">
         <v>383</v>
       </c>
-      <c r="C94" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
+      <c r="C182" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="183"/>
+    <row r="184">
+      <c r="A184" t="s" s="101">
         <v>467</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B184" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C184" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="B185" t="s">
         <v>385</v>
       </c>
-      <c r="C95" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>467</v>
-      </c>
-      <c r="B96" t="s">
+      <c r="C185" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="B186" t="s">
         <v>386</v>
       </c>
-      <c r="C96" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
+      <c r="C186" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="187"/>
+    <row r="188">
+      <c r="A188" t="s" s="101">
         <v>468</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B188" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C188" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" t="s">
         <v>388</v>
       </c>
-      <c r="C97" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>468</v>
-      </c>
-      <c r="B98" t="s">
+      <c r="C189" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" t="s">
         <v>389</v>
       </c>
-      <c r="C98" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>468</v>
-      </c>
-      <c r="B99" t="s">
+      <c r="C190" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" t="s">
         <v>390</v>
       </c>
-      <c r="C99" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>468</v>
-      </c>
-      <c r="B100" t="s">
+      <c r="C191" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" t="s">
         <v>391</v>
       </c>
-      <c r="C100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
-        <v>468</v>
-      </c>
-      <c r="B101" t="s">
+      <c r="C192" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" t="s">
         <v>392</v>
       </c>
-      <c r="C101" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>468</v>
-      </c>
-      <c r="B102" t="s">
+      <c r="C193" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="B194" t="s">
         <v>393</v>
       </c>
-      <c r="C102" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>468</v>
-      </c>
-      <c r="B103" t="s">
+      <c r="C194" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" t="s">
         <v>394</v>
       </c>
-      <c r="C103" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s">
+      <c r="C195" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="196"/>
+    <row r="197">
+      <c r="A197" t="s" s="101">
         <v>469</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B197" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C197" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="B198" t="s">
         <v>396</v>
       </c>
-      <c r="C104" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>469</v>
-      </c>
-      <c r="B105" t="s">
+      <c r="C198" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="B199" t="s">
         <v>397</v>
       </c>
-      <c r="C105" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>469</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="C199" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="B200" t="s">
         <v>398</v>
       </c>
-      <c r="C106" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s">
-        <v>469</v>
-      </c>
-      <c r="B107" t="s">
+      <c r="C200" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="B201" t="s">
         <v>399</v>
       </c>
-      <c r="C107" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s">
+      <c r="C201" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="202"/>
+    <row r="203">
+      <c r="A203" t="s" s="101">
         <v>470</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B203" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C203" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="B204" t="s">
         <v>376</v>
       </c>
-      <c r="C108" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
+      <c r="C204" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="B205" t="s">
+        <v>401</v>
+      </c>
+      <c r="C205" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="B206" t="s">
+        <v>402</v>
+      </c>
+      <c r="C206" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="B207" t="s">
+        <v>403</v>
+      </c>
+      <c r="C207" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="B208" t="s">
+        <v>404</v>
+      </c>
+      <c r="C208" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="B209" t="s">
+        <v>405</v>
+      </c>
+      <c r="C209" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="B210" t="s">
+        <v>406</v>
+      </c>
+      <c r="C210" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="B211" t="s">
+        <v>407</v>
+      </c>
+      <c r="C211" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="212"/>
+    <row r="213">
+      <c r="A213" t="s" s="101">
+        <v>471</v>
+      </c>
+      <c r="B213" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C213" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="B214" t="s">
+        <v>409</v>
+      </c>
+      <c r="C214" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="B215" t="s">
+        <v>410</v>
+      </c>
+      <c r="C215" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="216"/>
+    <row r="217">
+      <c r="A217" t="s" s="101">
         <v>470</v>
       </c>
-      <c r="B109" t="s">
-        <v>401</v>
-      </c>
-      <c r="C109" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s">
-        <v>470</v>
-      </c>
-      <c r="B110" t="s">
-        <v>402</v>
-      </c>
-      <c r="C110" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="s">
-        <v>470</v>
-      </c>
-      <c r="B111" t="s">
-        <v>403</v>
-      </c>
-      <c r="C111" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s">
-        <v>470</v>
-      </c>
-      <c r="B112" t="s">
-        <v>404</v>
-      </c>
-      <c r="C112" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="s">
-        <v>470</v>
-      </c>
-      <c r="B113" t="s">
-        <v>405</v>
-      </c>
-      <c r="C113" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="s">
-        <v>470</v>
-      </c>
-      <c r="B114" t="s">
-        <v>406</v>
-      </c>
-      <c r="C114" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="s">
-        <v>470</v>
-      </c>
-      <c r="B115" t="s">
-        <v>407</v>
-      </c>
-      <c r="C115" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="s">
-        <v>471</v>
-      </c>
-      <c r="B116" t="s">
-        <v>409</v>
-      </c>
-      <c r="C116" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="s">
-        <v>471</v>
-      </c>
-      <c r="B117" t="s">
-        <v>410</v>
-      </c>
-      <c r="C117" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="s">
-        <v>470</v>
-      </c>
-      <c r="B118" t="s">
+      <c r="B217" t="s" s="101">
+        <v>1</v>
+      </c>
+      <c r="C217" t="s" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="B218" t="s">
         <v>411</v>
       </c>
-      <c r="C118" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="s">
-        <v>470</v>
-      </c>
-      <c r="B119" t="s">
+      <c r="C218" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="B219" t="s">
         <v>412</v>
       </c>
-      <c r="C119" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="s">
-        <v>470</v>
-      </c>
-      <c r="B120" t="s">
+      <c r="C219" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="B220" t="s">
         <v>413</v>
       </c>
-      <c r="C120" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="s">
-        <v>470</v>
-      </c>
-      <c r="B121" t="s">
+      <c r="C220" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="B221" t="s">
         <v>414</v>
       </c>
-      <c r="C121" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="s">
-        <v>470</v>
-      </c>
-      <c r="B122" t="s">
+      <c r="C221" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="B222" t="s">
         <v>415</v>
       </c>
-      <c r="C122" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="s">
-        <v>470</v>
-      </c>
-      <c r="B123" t="s">
+      <c r="C222" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="B223" t="s">
         <v>416</v>
       </c>
-      <c r="C123" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="s">
-        <v>470</v>
-      </c>
-      <c r="B124" t="s">
+      <c r="C223" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="B224" t="s">
         <v>417</v>
       </c>
-      <c r="C124" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="s">
-        <v>470</v>
-      </c>
-      <c r="B125" t="s">
+      <c r="C224" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="B225" t="s">
         <v>418</v>
       </c>
-      <c r="C125" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="s">
-        <v>470</v>
-      </c>
-      <c r="B126" t="s">
+      <c r="C225" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="B226" t="s">
         <v>419</v>
       </c>
-      <c r="C126" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s">
-        <v>470</v>
-      </c>
-      <c r="B127" t="s">
+      <c r="C226" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="B227" t="s">
         <v>420</v>
       </c>
-      <c r="C127" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s">
-        <v>470</v>
-      </c>
-      <c r="B128" t="s">
+      <c r="C227" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="B228" t="s">
         <v>421</v>
       </c>
-      <c r="C128" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="s">
-        <v>470</v>
-      </c>
-      <c r="B129" t="s">
+      <c r="C228" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="B229" t="s">
         <v>422</v>
       </c>
-      <c r="C129" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="s">
-        <v>470</v>
-      </c>
-      <c r="B130" t="s">
+      <c r="C229" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="B230" t="s">
         <v>423</v>
       </c>
-      <c r="C130" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="s">
-        <v>470</v>
-      </c>
-      <c r="B131" t="s">
+      <c r="C230" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="B231" t="s">
         <v>424</v>
       </c>
-      <c r="C131" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="s">
-        <v>470</v>
-      </c>
-      <c r="B132" t="s">
+      <c r="C231" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="B232" t="s">
         <v>425</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C232" t="s">
         <v>255</v>
       </c>
     </row>

</xml_diff>